<commit_message>
* Worksheet will create if not there so no need to create sheet manually. * No will save as entry if no log files found.
</commit_message>
<xml_diff>
--- a/SujaiLogFile-1.xlsx
+++ b/SujaiLogFile-1.xlsx
@@ -1,22 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27809"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbalan/ZProjects/SujaiProject/logsToExcel/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1080" windowWidth="28160" windowHeight="14900" activeTab="2"/>
+    <workbookView xWindow="640" yWindow="1080" windowWidth="28160" windowHeight="14900" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="2" name="Apr" r:id="rId4"/>
-    <sheet sheetId="1" name="May" r:id="rId5"/>
-    <sheet sheetId="3" name="Jun" r:id="rId6"/>
+    <sheet name="Apr" sheetId="2" r:id="rId1"/>
+    <sheet name="May" sheetId="1" r:id="rId2"/>
+    <sheet name="Jun" sheetId="3" r:id="rId3"/>
+    <sheet name="Aug" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="24">
   <si>
     <t>10-May-2018</t>
   </si>
@@ -71,25 +85,54 @@
   <si>
     <t>2018-04-17 07:52:36 sinequa.connector.db error (2018-04-17 07:52:36) : 13 min 18 s 469 ms</t>
   </si>
+  <si>
+    <t>16-Aug-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>2018-08-16 07:39:22 error : compilation of '_WebAppHtmlTemplates.dll' failed : 5 error(s)
+f:\Sinequa\local-data\plugins\build\_WebAppHtmlTemplates\_v10_Box_Tree.cs(29,13) : error CS1061: 'Sinequa.Configuration.CCBox' does not contain a definition for 'TreeAsyncInitialLoad' and no extension method 'TreeAsyncInitialLoad' accepting a first argument of type 'Sinequa.Configuration.CCBox' could be found (are you missing a using directive or an assembly reference?)
+f:\Sinequa\local-data\plugins\build\_WebAppHtmlTemplates\_v10_Box_Tree_v2.cs(29,13) : error CS1061: 'Sinequa.Configuration.CCBox' does not contain a definition for 'TreeAsyncInitialLoad' and no extension method 'TreeAsyncInitialLoad' accepting a first argument of type 'Sinequa.Configuration.CCBox' could be found (are you missing a using directive or an assembly reference?)
+f:\Sinequa\local-data\plugins\build\_WebAppHtmlTemplates\_v10_ResultsView_List.cs(64,67) : error CS1501: No overload for method 'GetActionStatus' takes 5 arguments
+f:\Sinequa\local-data\plugins\build\_WebAppHtmlTemplates\_v10_ResultsView_List.cs(66,70) : error CS1061: 'Sinequa.Search.Doc' does not contain a definition for 'AuditEvent' and no extension method 'AuditEvent' accepting a first argument of type 'Sinequa.Search.Doc' could be found (are you missing a using directive or an assembly reference?)
+f:\Sinequa\local-data\plugins\build\_WebAppHtmlTemplates\_v10_ResultsView_List.cs(89,18) : error CS1501:</t>
+  </si>
+  <si>
+    <t>2018-08-16 07:52:36 WARNING : connector errors -&gt; Delete cancelled</t>
+  </si>
+  <si>
+    <t>2018-08-16 07:52:36           check 'Allow deletion on errors' in the advanced tab of your collection ('/DB/GPC2/') if you want to delete anyway</t>
+  </si>
+  <si>
+    <t>2018-08-16 07:52:36 indexing collection DB/GPC2 finished with error(s) : 13 min 13 s 47 ms</t>
+  </si>
+  <si>
+    <t>2018-08-16 07:52:36     0 document(s) in error</t>
+  </si>
+  <si>
+    <t>2018-08-16 07:52:36 sinequa.connector.db error (2018-08-16 07:52:36) : 13 min 18 s 469 ms</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <sz val="16"/>
       <color theme="0"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="16"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -115,24 +158,40 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium"/>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
       <right/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -438,30 +497,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" customWidth="1"/>
-    <col min="3" max="3" width="104.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" ht="43" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>7</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -473,22 +524,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="104.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+    <row r="1" spans="1:4" ht="43" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -500,11 +559,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="92.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -518,7 +581,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -532,7 +595,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -546,7 +609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -560,7 +623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -574,7 +637,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -588,7 +651,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -602,7 +665,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -616,7 +679,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -630,7 +693,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -644,7 +707,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -658,7 +721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -672,7 +735,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -686,7 +749,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -700,7 +763,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -714,7 +777,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -728,7 +791,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -742,7 +805,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -756,7 +819,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -770,7 +833,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -784,7 +847,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -798,7 +861,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -812,7 +875,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -826,7 +889,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -840,7 +903,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -854,7 +917,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -868,7 +931,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -882,7 +945,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -896,7 +959,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -910,7 +973,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -927,4 +990,119 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="255.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+</worksheet>
 </file>
</xml_diff>